<commit_message>
Product Def and Feature block diagram
</commit_message>
<xml_diff>
--- a/Douglas/Hours Tracking.xlsx
+++ b/Douglas/Hours Tracking.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17220" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -43,13 +38,43 @@
   </si>
   <si>
     <t>Actual</t>
+  </si>
+  <si>
+    <t>Feature Block Diagram</t>
+  </si>
+  <si>
+    <t>Product Definition.txt</t>
+  </si>
+  <si>
+    <t>Figure out illustrator</t>
+  </si>
+  <si>
+    <t>Place Objets</t>
+  </si>
+  <si>
+    <t>place relations</t>
+  </si>
+  <si>
+    <t>save as pdf</t>
+  </si>
+  <si>
+    <t>sync</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Fill out Text</t>
+  </si>
+  <si>
+    <t>Save</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -79,6 +104,22 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -97,10 +138,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -110,12 +157,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,19 +501,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.25" customWidth="1"/>
+    <col min="2" max="2" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16">
+    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +526,7 @@
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" ht="16">
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -475,16 +537,17 @@
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -505,30 +568,120 @@
       </c>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5">
+        <v>15</v>
+      </c>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
       <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>SUM(E5:E9)</f>
+        <v>37</v>
+      </c>
+      <c r="F10" s="7">
+        <f>SUM(F5:F9)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>